<commit_message>
final status of files at the start of day2
Files updated due to recap
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -153,7 +153,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -181,376 +181,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -699,7 +329,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E3:H13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -799,7 +429,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" numFmtId="14" showAll="0"/>
@@ -1122,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1345,9 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1385,10 +1013,11 @@
         <v>100000</v>
       </c>
       <c r="E2">
+        <f>C2-D2</f>
         <v>0</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(E2=0,"closed",IF(D2=0,"pending","open"))</f>
+        <f t="shared" ref="F2:F10" si="0">IF(E2=0,"closed",IF(D2=0,"pending","open"))</f>
         <v>closed</v>
       </c>
     </row>
@@ -1406,10 +1035,11 @@
         <v>80000</v>
       </c>
       <c r="E3">
+        <f>C3-D3</f>
         <v>0</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(E3=0,"closed",IF(D3=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>closed</v>
       </c>
     </row>
@@ -1427,10 +1057,11 @@
         <v>75000</v>
       </c>
       <c r="E4">
+        <f>C4-D4</f>
         <v>15000</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(E4=0,"closed",IF(D4=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>open</v>
       </c>
     </row>
@@ -1448,10 +1079,11 @@
         <v>35000</v>
       </c>
       <c r="E5">
+        <f>C5-D5</f>
         <v>20000</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(E5=0,"closed",IF(D5=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>open</v>
       </c>
     </row>
@@ -1469,10 +1101,11 @@
         <v>25000</v>
       </c>
       <c r="E6">
+        <f>C6-D6</f>
         <v>100000</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(E6=0,"closed",IF(D6=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>open</v>
       </c>
     </row>
@@ -1490,10 +1123,11 @@
         <v>0</v>
       </c>
       <c r="E7">
+        <f>C7-D7</f>
         <v>75000</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(E7=0,"closed",IF(D7=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>pending</v>
       </c>
     </row>
@@ -1511,10 +1145,11 @@
         <v>0</v>
       </c>
       <c r="E8">
+        <f>C8-D8</f>
         <v>89000</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(E8=0,"closed",IF(D8=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>pending</v>
       </c>
     </row>
@@ -1532,10 +1167,11 @@
         <v>50000</v>
       </c>
       <c r="E9">
+        <f>C9-D9</f>
         <v>3000</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(E9=0,"closed",IF(D9=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>open</v>
       </c>
     </row>
@@ -1553,22 +1189,23 @@
         <v>20000</v>
       </c>
       <c r="E10">
+        <f>C10-D10</f>
         <v>0</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(E10=0,"closed",IF(D10=0,"pending","open"))</f>
+        <f t="shared" si="0"/>
         <v>closed</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="containsText" dxfId="29" priority="1" operator="containsText" text="closed">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="closed">
       <formula>NOT(ISERROR(SEARCH("closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="pending">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pending">
       <formula>NOT(ISERROR(SEARCH("pending",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="open">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="open">
       <formula>NOT(ISERROR(SEARCH("open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>